<commit_message>
Add 12MHz crystal support
</commit_message>
<xml_diff>
--- a/MCP2515Calc.xlsx
+++ b/MCP2515Calc.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr checkCompatibility="1" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncang/Documents/GitHub/MCP_CAN_lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D227DB9-E0C3-DB40-A872-457A81BF0B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6135"/>
+    <workbookView xWindow="3220" yWindow="3140" windowWidth="25140" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -238,7 +251,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0\x##"/>
   </numFmts>
@@ -1481,7 +1494,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1489,156 +1502,272 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1647,181 +1776,45 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Green" xfId="1"/>
-    <cellStyle name="Heading" xfId="2"/>
-    <cellStyle name="Heading1" xfId="3"/>
+    <cellStyle name="Green" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading1" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Red" xfId="4"/>
-    <cellStyle name="Result" xfId="5"/>
-    <cellStyle name="Result2" xfId="6"/>
+    <cellStyle name="Red" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Result" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Result2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2106,269 +2099,269 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="1024" width="10.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="1024" width="10.6640625" style="1" customWidth="1"/>
     <col min="1025" max="1025" width="9" style="1"/>
     <col min="1026" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="17"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="68"/>
     </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="19">
-        <v>16</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="4">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="21" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="23"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="51"/>
     </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25">
-        <v>250</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="7">
+        <v>125</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29">
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="9">
         <v>1</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="29">
+      <c r="I3" s="59"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36" t="s">
+    <row r="4" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38">
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="13">
         <v>1</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="40"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="38">
+      <c r="I4" s="56"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="14">
         <f>(2*(B8+1))/B2</f>
-        <v>0.25</v>
-      </c>
-      <c r="C5" s="26" t="s">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38">
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="13">
         <v>6</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="40"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="38">
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+    <row r="6" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="16">
         <f>(1/B3)*1000</f>
-        <v>4</v>
-      </c>
-      <c r="C6" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="48">
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="18">
         <v>5</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="50"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52">
+      <c r="I6" s="53"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="16">
         <f>B6/B5</f>
-        <v>16</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="52">
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="19">
         <v>1</v>
       </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="58">
+      <c r="B8" s="16">
         <f>BIN2DEC(CONCATENATE(F15,G15,H15,I15,J15,K15))+0</f>
         <v>1</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="62"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
     </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63" t="s">
+    <row r="9" spans="1:16" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="64">
+      <c r="B9" s="23">
         <f>BIN2DEC(CONCATENATE(D15,E15))+1</f>
         <v>2</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="60" t="s">
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="70"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72" t="s">
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="74"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="90"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="57" t="s">
+    <row r="11" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="16">
         <f>BIN2DEC(CONCATENATE(I17,J17,K17))+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="24" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="75" t="s">
@@ -2376,318 +2369,319 @@
       </c>
       <c r="E11" s="76"/>
       <c r="F11" s="77"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="78"/>
-      <c r="K11" s="79"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="57" t="s">
+    <row r="12" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="58">
+      <c r="B12" s="16">
         <f>BIN2DEC(CONCATENATE(F17,G17,H17))+1</f>
         <v>7</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="80" t="s">
+      <c r="D12" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="82"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="68"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="58">
+      <c r="B13" s="16">
         <f>BIN2DEC(CONCATENATE(I19,J19,K19))+1</f>
         <v>6</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="84"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="86" t="s">
+      <c r="E13" s="93"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="26" t="s">
         <v>18</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="87"/>
-      <c r="B14" s="88">
+    <row r="14" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28">
         <f>SUM(B10:B13)</f>
         <v>16</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="90">
+      <c r="D14" s="30">
         <v>7</v>
       </c>
-      <c r="E14" s="91">
+      <c r="E14" s="31">
         <v>6</v>
       </c>
-      <c r="F14" s="91">
+      <c r="F14" s="31">
         <v>5</v>
       </c>
-      <c r="G14" s="91">
+      <c r="G14" s="31">
         <v>4</v>
       </c>
-      <c r="H14" s="91">
+      <c r="H14" s="31">
         <v>3</v>
       </c>
-      <c r="I14" s="91">
+      <c r="I14" s="31">
         <v>2</v>
       </c>
-      <c r="J14" s="91">
+      <c r="J14" s="31">
         <v>1</v>
       </c>
-      <c r="K14" s="92">
+      <c r="K14" s="32">
         <v>0</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:16" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="12" t="str">
+      <c r="B15" s="86" t="str">
         <f>BIN2HEX(C15)</f>
         <v>41</v>
       </c>
-      <c r="C15" s="5" t="str">
+      <c r="C15" s="84" t="str">
         <f>CONCATENATE(D15,E15,F15,G15,H15,I15,J15,K15)</f>
         <v>01000001</v>
       </c>
-      <c r="D15" s="93" t="str">
+      <c r="D15" s="33" t="str">
         <f>MID(DEC2BIN(G7,2),1,1)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="94" t="str">
+      <c r="E15" s="34" t="str">
         <f>MID(DEC2BIN(G7,2),2,1)</f>
         <v>1</v>
       </c>
-      <c r="F15" s="93" t="str">
+      <c r="F15" s="33" t="str">
         <f>MID(DEC2BIN(G3,8),3,1)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="95" t="str">
+      <c r="G15" s="35" t="str">
         <f>MID(DEC2BIN(G3,8),4,1)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="95" t="str">
+      <c r="H15" s="35" t="str">
         <f>MID(DEC2BIN(G3,8),5,1)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="95" t="str">
+      <c r="I15" s="35" t="str">
         <f>MID(DEC2BIN(G3,8),6,1)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="95" t="str">
+      <c r="J15" s="35" t="str">
         <f>MID(DEC2BIN(G3,8),7,1)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="96" t="str">
+      <c r="K15" s="36" t="str">
         <f>MID(DEC2BIN(G3,8),8,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="97" t="s">
+    <row r="16" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="83"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="98"/>
-      <c r="F16" s="97" t="s">
+      <c r="E16" s="79"/>
+      <c r="F16" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="100"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="81"/>
     </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8" t="str">
+      <c r="B17" s="104" t="str">
         <f t="shared" ref="B17" si="0">BIN2HEX(C17)</f>
         <v>F1</v>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C17" s="84" t="str">
         <f t="shared" ref="C17" si="1">CONCATENATE(D17,E17,F17,G17,H17,I17,J17,K17)</f>
         <v>11110001</v>
       </c>
-      <c r="D17" s="101" t="str">
+      <c r="D17" s="37" t="str">
         <f>MID(DEC2BIN(K3,1),1,1)</f>
         <v>1</v>
       </c>
-      <c r="E17" s="101" t="str">
+      <c r="E17" s="37" t="str">
         <f>MID(DEC2BIN(K4,1),1,1)</f>
         <v>1</v>
       </c>
-      <c r="F17" s="102" t="str">
+      <c r="F17" s="38" t="str">
         <f>MID(DEC2BIN(G5,3),1,1)</f>
         <v>1</v>
       </c>
-      <c r="G17" s="103" t="str">
+      <c r="G17" s="39" t="str">
         <f>MID(DEC2BIN(G5,3),2,1)</f>
         <v>1</v>
       </c>
-      <c r="H17" s="104" t="str">
+      <c r="H17" s="40" t="str">
         <f>MID(DEC2BIN(G5,3),3,1)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="105" t="str">
+      <c r="I17" s="41" t="str">
         <f>MID(DEC2BIN(G4,3),1,1)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="103" t="str">
+      <c r="J17" s="39" t="str">
         <f>MID(DEC2BIN(G4,3),2,1)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="106" t="str">
+      <c r="K17" s="42" t="str">
         <f>MID(DEC2BIN(G4,3),3,1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="107" t="s">
+    <row r="18" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="83"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="107" t="s">
+      <c r="E18" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="97" t="s">
+      <c r="F18" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="99"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="108" t="s">
+      <c r="G18" s="80"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="99"/>
-      <c r="K18" s="100"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="81"/>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8" t="str">
+      <c r="B19" s="104" t="str">
         <f t="shared" ref="B19" si="2">BIN2HEX(C19)</f>
         <v>85</v>
       </c>
-      <c r="C19" s="5" t="str">
+      <c r="C19" s="84" t="str">
         <f t="shared" ref="C19" si="3">CONCATENATE(D19,E19,F19,G19,H19,I19,J19,K19)</f>
         <v>10000101</v>
       </c>
-      <c r="D19" s="109" t="str">
+      <c r="D19" s="44" t="str">
         <f>MID(DEC2BIN(K5,1),1,1)</f>
         <v>1</v>
       </c>
-      <c r="E19" s="109" t="str">
+      <c r="E19" s="44" t="str">
         <f>MID(DEC2BIN(K6,1),1,1)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="102">
+      <c r="F19" s="38">
         <v>0</v>
       </c>
-      <c r="G19" s="103">
+      <c r="G19" s="39">
         <v>0</v>
       </c>
-      <c r="H19" s="104">
+      <c r="H19" s="40">
         <v>0</v>
       </c>
-      <c r="I19" s="102" t="str">
+      <c r="I19" s="38" t="str">
         <f>MID(DEC2BIN(G6,8),6,1)</f>
         <v>1</v>
       </c>
-      <c r="J19" s="103" t="str">
+      <c r="J19" s="39" t="str">
         <f>MID(DEC2BIN(G6,8),7,1)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="106" t="str">
+      <c r="K19" s="42" t="str">
         <f>MID(DEC2BIN(G6,8),8,1)</f>
         <v>1</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="110" t="s">
+    <row r="20" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="102"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="110" t="s">
+      <c r="E20" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="111" t="s">
+      <c r="F20" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="G20" s="112"/>
-      <c r="H20" s="113"/>
-      <c r="I20" s="111" t="s">
+      <c r="G20" s="99"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="112"/>
-      <c r="K20" s="114"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="101"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D8:K8"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
@@ -2704,16 +2698,15 @@
     <mergeCell ref="E13:J13"/>
     <mergeCell ref="G9:K9"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D2:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="B14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">

</xml_diff>